<commit_message>
Os experimentos envolvendo o Sammon’s mapping foram finalizados; Alguns bugs nos scripts de armazenamento e processamento dos resultados foram corrigidos;
</commit_message>
<xml_diff>
--- a/PaperNeural/Results/ResultsMar2017-Sammon_MI_4000_LR_0.5.xlsx
+++ b/PaperNeural/Results/ResultsMar2017-Sammon_MI_4000_LR_0.5.xlsx
@@ -7464,34 +7464,56 @@
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>31.57894736842105</v>
+      </c>
       <c r="I18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>11.695906432748536</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -7500,9 +7522,15 @@
       <c r="I19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -7514,9 +7542,15 @@
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.5</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -7525,9 +7559,15 @@
       <c r="I20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.09259259259259259</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.9074074074074074</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -7598,34 +7638,56 @@
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>29.239766081871345</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.375</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -7634,9 +7696,15 @@
       <c r="I25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -7648,9 +7716,15 @@
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -7659,9 +7733,15 @@
       <c r="I26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.3148148148148148</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.6851851851851852</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -8175,34 +8255,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.2</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>47.368421052631575</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.044444444444444446</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>33.91812865497076</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -8211,9 +8313,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.1527777777777778</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -8225,9 +8333,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -8236,9 +8350,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.7222222222222222</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -8309,34 +8429,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.4</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>42.10526315789473</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.7555555555555555</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.08888888888888889</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>27.485380116959064</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -8345,9 +8487,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.06944444444444445</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.7361111111111112</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.19444444444444445</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -8359,9 +8507,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.5</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -8370,9 +8524,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.09259259259259259</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.6851851851851852</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -8886,34 +9046,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>15.789473684210526</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>11.11111111111111</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -8922,9 +9104,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.8611111111111112</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -8936,9 +9124,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -8947,9 +9141,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.8888888888888888</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -9020,34 +9220,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>31.57894736842105</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.8222222222222222</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.08888888888888889</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>26.900584795321635</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -9056,9 +9278,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.041666666666666664</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -9070,9 +9298,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -9081,9 +9315,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.09259259259259259</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.6296296296296297</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -9597,34 +9837,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>15.789473684210526</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.6444444444444445</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>23.391812865497073</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -9633,9 +9895,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -9647,9 +9915,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -9658,9 +9932,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.8518518518518519</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -9731,34 +10011,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.2</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>23.391812865497073</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -9767,9 +10069,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.06944444444444445</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.7361111111111112</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.19444444444444445</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -9781,9 +10089,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>1.0</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -9792,9 +10106,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.7037037037037037</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -10304,34 +10624,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>31.57894736842105</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>14.035087719298245</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -10340,9 +10682,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.8611111111111112</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -10354,9 +10702,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -10365,9 +10719,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.8703703703703703</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -10438,34 +10798,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>26.31578947368421</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>23.391812865497073</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -10474,9 +10856,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.2222222222222222</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -10488,9 +10876,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -10499,9 +10893,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.7037037037037037</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -11015,34 +11415,56 @@
       <c r="B18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.6222222222222222</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.044444444444444446</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>24.561403508771928</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -11051,9 +11473,15 @@
       <c r="I19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -11065,9 +11493,15 @@
       <c r="B20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -11076,9 +11510,15 @@
       <c r="I20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -11149,34 +11589,56 @@
       <c r="B24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>15.789473684210526</v>
+      </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>21.637426900584796</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -11185,9 +11647,15 @@
       <c r="I25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.18055555555555555</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -11199,9 +11667,15 @@
       <c r="B26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -11210,9 +11684,15 @@
       <c r="I26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.24074074074074073</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.7592592592592593</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -11561,34 +12041,56 @@
       <c r="B12" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="C12" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E12" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F12" s="3" t="e">
         <f>100*C12/SUM(C12:E12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G12" s="63"/>
+      <c r="G12" s="63" t="n">
+        <v>26.31578947368421</v>
+      </c>
       <c r="I12" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
+      <c r="J12" s="40" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="K12" s="40" t="n">
+        <v>0.044444444444444446</v>
+      </c>
+      <c r="L12" s="40" t="n">
+        <v>0.08888888888888889</v>
+      </c>
       <c r="M12" s="3" t="e">
         <f>100*J12/(SUM(J12:L12))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N12" s="63"/>
+      <c r="N12" s="63" t="n">
+        <v>16.374269005847953</v>
+      </c>
     </row>
     <row r="13" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="61"/>
       <c r="B13" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="C13" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D13" s="40" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E13" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
         <v>#DIV/0!</v>
@@ -11597,9 +12099,15 @@
       <c r="I13" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
+      <c r="J13" s="40" t="n">
+        <v>0.041666666666666664</v>
+      </c>
+      <c r="K13" s="40" t="n">
+        <v>0.8611111111111112</v>
+      </c>
+      <c r="L13" s="40" t="n">
+        <v>0.09722222222222222</v>
+      </c>
       <c r="M13" s="3" t="e">
         <f>100*K13/(SUM(J13:L13))</f>
         <v>#DIV/0!</v>
@@ -11611,9 +12119,15 @@
       <c r="B14" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="C14" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E14" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F14" s="3" t="e">
         <f>100*E14/SUM(C14:E14)</f>
         <v>#DIV/0!</v>
@@ -11622,9 +12136,15 @@
       <c r="I14" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
+      <c r="J14" s="40" t="n">
+        <v>0.07407407407407407</v>
+      </c>
+      <c r="K14" s="40" t="n">
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="L14" s="40" t="n">
+        <v>0.7777777777777778</v>
+      </c>
       <c r="M14" s="3" t="e">
         <f>100*L14/(SUM(J14:L14))</f>
         <v>#DIV/0!</v>
@@ -11695,34 +12215,56 @@
       <c r="B18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>19.883040935672515</v>
+      </c>
     </row>
     <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -11731,9 +12273,15 @@
       <c r="I19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.7361111111111112</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -11745,9 +12293,15 @@
       <c r="B20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -11756,9 +12310,15 @@
       <c r="I20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.09259259259259259</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.9074074074074074</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -11829,34 +12389,56 @@
       <c r="B24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>36.84210526315789</v>
+      </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>23.391812865497073</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -11865,9 +12447,15 @@
       <c r="I25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.7361111111111112</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -11879,9 +12467,15 @@
       <c r="B26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.5</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -11890,9 +12484,15 @@
       <c r="I26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.7222222222222222</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>

</xml_diff>